<commit_message>
test cases and fixes
</commit_message>
<xml_diff>
--- a/src/main/resources/EpocSettings.xlsx
+++ b/src/main/resources/EpocSettings.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="81">
   <si>
     <t>settingKey</t>
   </si>
@@ -121,72 +121,75 @@
     <t>SET0011</t>
   </si>
   <si>
+    <t>CHF 500000</t>
+  </si>
+  <si>
+    <t>Unit labour cost per production line and year</t>
+  </si>
+  <si>
+    <t>SET0012</t>
+  </si>
+  <si>
+    <t>CHF 10000</t>
+  </si>
+  <si>
+    <t>Building maintenance per year and building</t>
+  </si>
+  <si>
+    <t>SET0013</t>
+  </si>
+  <si>
+    <t>Percent</t>
+  </si>
+  <si>
+    <t>5%</t>
+  </si>
+  <si>
+    <t>Credit line interest rate</t>
+  </si>
+  <si>
+    <t>SET0014</t>
+  </si>
+  <si>
+    <t>CHF 35</t>
+  </si>
+  <si>
+    <t>Unit price for raw material</t>
+  </si>
+  <si>
+    <t>SET0015</t>
+  </si>
+  <si>
+    <t>20%</t>
+  </si>
+  <si>
+    <t>Demand higher percent</t>
+  </si>
+  <si>
+    <t>SET0016</t>
+  </si>
+  <si>
+    <t>CHF 80</t>
+  </si>
+  <si>
+    <t>Demand higher price</t>
+  </si>
+  <si>
+    <t>SET0017</t>
+  </si>
+  <si>
+    <t>80%</t>
+  </si>
+  <si>
+    <t>Demand lower percent</t>
+  </si>
+  <si>
+    <t>SET0018</t>
+  </si>
+  <si>
     <t>CHF 20</t>
   </si>
   <si>
-    <t>Unit labour cost</t>
-  </si>
-  <si>
-    <t>SET0012</t>
-  </si>
-  <si>
-    <t>CHF 10000</t>
-  </si>
-  <si>
-    <t>Building maintenance per year and building</t>
-  </si>
-  <si>
-    <t>SET0013</t>
-  </si>
-  <si>
-    <t>Percent</t>
-  </si>
-  <si>
-    <t>5%</t>
-  </si>
-  <si>
-    <t>Credit line interest rate</t>
-  </si>
-  <si>
-    <t>SET0014</t>
-  </si>
-  <si>
-    <t>CHF 35</t>
-  </si>
-  <si>
-    <t>Unit price for raw material</t>
-  </si>
-  <si>
-    <t>SET0015</t>
-  </si>
-  <si>
-    <t>20%</t>
-  </si>
-  <si>
-    <t>Demand higher percent</t>
-  </si>
-  <si>
-    <t>SET0016</t>
-  </si>
-  <si>
-    <t>CHF 80</t>
-  </si>
-  <si>
-    <t>Demand higher price</t>
-  </si>
-  <si>
-    <t>SET0017</t>
-  </si>
-  <si>
-    <t>80%</t>
-  </si>
-  <si>
-    <t>Demand lower percent</t>
-  </si>
-  <si>
-    <t>SET0018</t>
-  </si>
-  <si>
     <t>Demand lower price</t>
   </si>
   <si>
@@ -199,9 +202,6 @@
     <t>SET0020</t>
   </si>
   <si>
-    <t>CHF 500000</t>
-  </si>
-  <si>
     <t>Fixed costs per market entry</t>
   </si>
   <si>
@@ -245,6 +245,15 @@
   </si>
   <si>
     <t>Headquarter cost per annum</t>
+  </si>
+  <si>
+    <t>SET0026</t>
+  </si>
+  <si>
+    <t>CHF 30</t>
+  </si>
+  <si>
+    <t>Own production cost</t>
   </si>
 </sst>
 </file>
@@ -254,7 +263,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -266,13 +275,18 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,8 +305,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -320,6 +340,19 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
@@ -365,6 +398,17 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
@@ -402,6 +446,19 @@
       </top>
       <bottom style="thin">
         <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -411,32 +468,41 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -459,6 +525,8 @@
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
   </colors>
@@ -476,10 +544,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -656,11 +724,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -669,33 +740,33 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -934,12 +1005,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1220,7 +1291,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1488,19 +1559,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="10" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.6719" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.3516" style="1" customWidth="1"/>
-    <col min="4" max="4" width="65.7188" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="4" max="4" width="65.6719" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -1516,356 +1586,397 @@
       <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="A2" t="s" s="4">
         <v>4</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="B2" t="s" s="5">
         <v>5</v>
       </c>
-      <c r="C2" t="s" s="5">
+      <c r="C2" t="s" s="6">
         <v>6</v>
       </c>
-      <c r="D2" t="s" s="5">
+      <c r="D2" t="s" s="6">
         <v>7</v>
       </c>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" t="s" s="6">
+      <c r="A3" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="B3" t="s" s="7">
+      <c r="B3" t="s" s="9">
         <v>5</v>
       </c>
-      <c r="C3" t="s" s="8">
+      <c r="C3" t="s" s="10">
         <v>9</v>
       </c>
-      <c r="D3" t="s" s="8">
+      <c r="D3" t="s" s="10">
         <v>10</v>
       </c>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="6">
+      <c r="A4" t="s" s="8">
         <v>11</v>
       </c>
-      <c r="B4" t="s" s="7">
+      <c r="B4" t="s" s="9">
         <v>5</v>
       </c>
-      <c r="C4" t="s" s="8">
+      <c r="C4" t="s" s="10">
         <v>6</v>
       </c>
-      <c r="D4" t="s" s="8">
+      <c r="D4" t="s" s="10">
         <v>12</v>
       </c>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="6">
+      <c r="A5" t="s" s="8">
         <v>13</v>
       </c>
-      <c r="B5" t="s" s="7">
+      <c r="B5" t="s" s="9">
         <v>5</v>
       </c>
-      <c r="C5" t="s" s="8">
+      <c r="C5" t="s" s="10">
         <v>14</v>
       </c>
-      <c r="D5" t="s" s="8">
+      <c r="D5" t="s" s="10">
         <v>15</v>
       </c>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="6">
+      <c r="A6" t="s" s="8">
         <v>16</v>
       </c>
-      <c r="B6" t="s" s="7">
+      <c r="B6" t="s" s="9">
         <v>17</v>
       </c>
-      <c r="C6" t="s" s="8">
+      <c r="C6" t="s" s="10">
         <v>18</v>
       </c>
-      <c r="D6" t="s" s="8">
+      <c r="D6" t="s" s="10">
         <v>19</v>
       </c>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="6">
+      <c r="A7" t="s" s="8">
         <v>20</v>
       </c>
-      <c r="B7" t="s" s="7">
+      <c r="B7" t="s" s="9">
         <v>17</v>
       </c>
-      <c r="C7" t="s" s="8">
+      <c r="C7" t="s" s="10">
         <v>21</v>
       </c>
-      <c r="D7" t="s" s="8">
+      <c r="D7" t="s" s="10">
         <v>22</v>
       </c>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="6">
+      <c r="A8" t="s" s="8">
         <v>23</v>
       </c>
-      <c r="B8" t="s" s="7">
+      <c r="B8" t="s" s="9">
         <v>17</v>
       </c>
-      <c r="C8" t="s" s="8">
+      <c r="C8" t="s" s="10">
         <v>21</v>
       </c>
-      <c r="D8" t="s" s="8">
+      <c r="D8" t="s" s="10">
         <v>24</v>
       </c>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" t="s" s="6">
+      <c r="A9" t="s" s="8">
         <v>25</v>
       </c>
-      <c r="B9" t="s" s="7">
+      <c r="B9" t="s" s="9">
         <v>17</v>
       </c>
-      <c r="C9" t="s" s="8">
+      <c r="C9" t="s" s="10">
         <v>26</v>
       </c>
-      <c r="D9" t="s" s="8">
+      <c r="D9" t="s" s="10">
         <v>27</v>
       </c>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" t="s" s="6">
+      <c r="A10" t="s" s="8">
         <v>28</v>
       </c>
-      <c r="B10" t="s" s="7">
+      <c r="B10" t="s" s="9">
         <v>29</v>
       </c>
-      <c r="C10" t="s" s="8">
+      <c r="C10" t="s" s="10">
         <v>30</v>
       </c>
-      <c r="D10" t="s" s="8">
+      <c r="D10" t="s" s="10">
         <v>31</v>
       </c>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" t="s" s="6">
+      <c r="A11" t="s" s="8">
         <v>32</v>
       </c>
-      <c r="B11" t="s" s="7">
+      <c r="B11" t="s" s="9">
         <v>5</v>
       </c>
-      <c r="C11" t="s" s="8">
+      <c r="C11" t="s" s="10">
         <v>33</v>
       </c>
-      <c r="D11" t="s" s="8">
+      <c r="D11" t="s" s="10">
         <v>34</v>
       </c>
+      <c r="E11" s="7"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" t="s" s="6">
+      <c r="A12" t="s" s="8">
         <v>35</v>
       </c>
-      <c r="B12" t="s" s="7">
+      <c r="B12" t="s" s="9">
         <v>5</v>
       </c>
-      <c r="C12" t="s" s="8">
+      <c r="C12" t="s" s="10">
         <v>36</v>
       </c>
-      <c r="D12" t="s" s="8">
+      <c r="D12" t="s" s="10">
         <v>37</v>
       </c>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" t="s" s="6">
+      <c r="A13" t="s" s="8">
         <v>38</v>
       </c>
-      <c r="B13" t="s" s="7">
+      <c r="B13" t="s" s="9">
         <v>5</v>
       </c>
-      <c r="C13" t="s" s="8">
+      <c r="C13" t="s" s="10">
         <v>39</v>
       </c>
-      <c r="D13" t="s" s="8">
+      <c r="D13" t="s" s="10">
         <v>40</v>
       </c>
+      <c r="E13" s="7"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" t="s" s="6">
+      <c r="A14" t="s" s="8">
         <v>41</v>
       </c>
-      <c r="B14" t="s" s="7">
+      <c r="B14" t="s" s="9">
         <v>42</v>
       </c>
-      <c r="C14" t="s" s="8">
+      <c r="C14" t="s" s="10">
         <v>43</v>
       </c>
-      <c r="D14" t="s" s="8">
+      <c r="D14" t="s" s="10">
         <v>44</v>
       </c>
+      <c r="E14" s="7"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" t="s" s="6">
+      <c r="A15" t="s" s="8">
         <v>45</v>
       </c>
-      <c r="B15" t="s" s="7">
+      <c r="B15" t="s" s="9">
         <v>5</v>
       </c>
-      <c r="C15" t="s" s="8">
+      <c r="C15" t="s" s="10">
         <v>46</v>
       </c>
-      <c r="D15" t="s" s="8">
+      <c r="D15" t="s" s="10">
         <v>47</v>
       </c>
+      <c r="E15" s="7"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" t="s" s="6">
+      <c r="A16" t="s" s="8">
         <v>48</v>
       </c>
-      <c r="B16" t="s" s="7">
+      <c r="B16" t="s" s="9">
         <v>42</v>
       </c>
-      <c r="C16" t="s" s="8">
+      <c r="C16" t="s" s="10">
         <v>49</v>
       </c>
-      <c r="D16" t="s" s="8">
+      <c r="D16" t="s" s="10">
         <v>50</v>
       </c>
+      <c r="E16" s="7"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" t="s" s="6">
+      <c r="A17" t="s" s="8">
         <v>51</v>
       </c>
-      <c r="B17" t="s" s="7">
+      <c r="B17" t="s" s="9">
         <v>5</v>
       </c>
-      <c r="C17" t="s" s="8">
+      <c r="C17" t="s" s="10">
         <v>52</v>
       </c>
-      <c r="D17" t="s" s="8">
+      <c r="D17" t="s" s="10">
         <v>53</v>
       </c>
+      <c r="E17" s="7"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" t="s" s="6">
+      <c r="A18" t="s" s="8">
         <v>54</v>
       </c>
-      <c r="B18" t="s" s="7">
+      <c r="B18" t="s" s="9">
         <v>42</v>
       </c>
-      <c r="C18" t="s" s="8">
+      <c r="C18" t="s" s="10">
         <v>55</v>
       </c>
-      <c r="D18" t="s" s="8">
+      <c r="D18" t="s" s="10">
         <v>56</v>
       </c>
+      <c r="E18" s="7"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" t="s" s="6">
+      <c r="A19" t="s" s="8">
         <v>57</v>
       </c>
-      <c r="B19" t="s" s="7">
+      <c r="B19" t="s" s="9">
         <v>5</v>
       </c>
-      <c r="C19" t="s" s="8">
+      <c r="C19" t="s" s="10">
+        <v>58</v>
+      </c>
+      <c r="D19" t="s" s="10">
+        <v>59</v>
+      </c>
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" ht="20.05" customHeight="1">
+      <c r="A20" t="s" s="8">
+        <v>60</v>
+      </c>
+      <c r="B20" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s" s="10">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s" s="10">
+        <v>61</v>
+      </c>
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" ht="20.05" customHeight="1">
+      <c r="A21" t="s" s="8">
+        <v>62</v>
+      </c>
+      <c r="B21" t="s" s="9">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s" s="10">
         <v>36</v>
       </c>
-      <c r="D19" t="s" s="8">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" t="s" s="6">
-        <v>59</v>
-      </c>
-      <c r="B20" t="s" s="7">
-        <v>17</v>
-      </c>
-      <c r="C20" t="s" s="8">
-        <v>18</v>
-      </c>
-      <c r="D20" t="s" s="8">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" t="s" s="6">
-        <v>61</v>
-      </c>
-      <c r="B21" t="s" s="7">
+      <c r="D21" t="s" s="10">
+        <v>63</v>
+      </c>
+      <c r="E21" s="7"/>
+    </row>
+    <row r="22" ht="20.05" customHeight="1">
+      <c r="A22" t="s" s="8">
+        <v>64</v>
+      </c>
+      <c r="B22" t="s" s="9">
         <v>5</v>
       </c>
-      <c r="C21" t="s" s="8">
-        <v>62</v>
-      </c>
-      <c r="D21" t="s" s="8">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" t="s" s="6">
-        <v>64</v>
-      </c>
-      <c r="B22" t="s" s="7">
+      <c r="C22" t="s" s="10">
+        <v>65</v>
+      </c>
+      <c r="D22" t="s" s="10">
+        <v>66</v>
+      </c>
+      <c r="E22" s="7"/>
+    </row>
+    <row r="23" ht="20.05" customHeight="1">
+      <c r="A23" t="s" s="8">
+        <v>67</v>
+      </c>
+      <c r="B23" t="s" s="9">
+        <v>68</v>
+      </c>
+      <c r="C23" t="s" s="10">
+        <v>69</v>
+      </c>
+      <c r="D23" t="s" s="10">
+        <v>70</v>
+      </c>
+      <c r="E23" s="7"/>
+    </row>
+    <row r="24" ht="20.05" customHeight="1">
+      <c r="A24" t="s" s="8">
+        <v>71</v>
+      </c>
+      <c r="B24" t="s" s="9">
+        <v>42</v>
+      </c>
+      <c r="C24" t="s" s="10">
+        <v>72</v>
+      </c>
+      <c r="D24" t="s" s="10">
+        <v>73</v>
+      </c>
+      <c r="E24" s="7"/>
+    </row>
+    <row r="25" ht="20.05" customHeight="1">
+      <c r="A25" t="s" s="8">
+        <v>74</v>
+      </c>
+      <c r="B25" t="s" s="9">
         <v>5</v>
       </c>
-      <c r="C22" t="s" s="8">
-        <v>65</v>
-      </c>
-      <c r="D22" t="s" s="8">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" t="s" s="6">
-        <v>67</v>
-      </c>
-      <c r="B23" t="s" s="7">
-        <v>68</v>
-      </c>
-      <c r="C23" t="s" s="8">
-        <v>69</v>
-      </c>
-      <c r="D23" t="s" s="8">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" t="s" s="6">
-        <v>71</v>
-      </c>
-      <c r="B24" t="s" s="7">
-        <v>42</v>
-      </c>
-      <c r="C24" t="s" s="8">
-        <v>72</v>
-      </c>
-      <c r="D24" t="s" s="8">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" ht="20.05" customHeight="1">
-      <c r="A25" t="s" s="6">
-        <v>74</v>
-      </c>
-      <c r="B25" t="s" s="7">
+      <c r="C25" t="s" s="10">
+        <v>36</v>
+      </c>
+      <c r="D25" t="s" s="10">
+        <v>75</v>
+      </c>
+      <c r="E25" s="7"/>
+    </row>
+    <row r="26" ht="20.05" customHeight="1">
+      <c r="A26" t="s" s="8">
+        <v>76</v>
+      </c>
+      <c r="B26" t="s" s="9">
         <v>5</v>
       </c>
-      <c r="C25" t="s" s="8">
-        <v>62</v>
-      </c>
-      <c r="D25" t="s" s="8">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" ht="20.05" customHeight="1">
-      <c r="A26" t="s" s="6">
-        <v>76</v>
-      </c>
-      <c r="B26" t="s" s="7">
+      <c r="C26" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s" s="10">
+        <v>77</v>
+      </c>
+      <c r="E26" s="7"/>
+    </row>
+    <row r="27" ht="20.05" customHeight="1">
+      <c r="A27" t="s" s="8">
+        <v>78</v>
+      </c>
+      <c r="B27" t="s" s="9">
         <v>5</v>
       </c>
-      <c r="C26" t="s" s="8">
-        <v>6</v>
-      </c>
-      <c r="D26" t="s" s="8">
-        <v>77</v>
-      </c>
+      <c r="C27" t="s" s="10">
+        <v>79</v>
+      </c>
+      <c r="D27" t="s" s="10">
+        <v>80</v>
+      </c>
+      <c r="E27" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>

<commit_message>
implemented simulation specific settings
</commit_message>
<xml_diff>
--- a/src/main/resources/EpocSettings.xlsx
+++ b/src/main/resources/EpocSettings.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="77">
   <si>
     <t>settingKey</t>
   </si>
@@ -76,7 +76,7 @@
     <t>SET0006</t>
   </si>
   <si>
-    <t>1</t>
+    <t>12</t>
   </si>
   <si>
     <t>Months required to construct a factory</t>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>SET0008</t>
-  </si>
-  <si>
-    <t>12</t>
   </si>
   <si>
     <t>Length of password in characters</t>
@@ -1710,151 +1707,151 @@
         <v>17</v>
       </c>
       <c r="C9" t="s" s="10">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s" s="10">
         <v>26</v>
-      </c>
-      <c r="D9" t="s" s="10">
-        <v>27</v>
       </c>
       <c r="E9" s="7"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s" s="9">
         <v>28</v>
       </c>
-      <c r="B10" t="s" s="9">
+      <c r="C10" t="s" s="10">
         <v>29</v>
       </c>
-      <c r="C10" t="s" s="10">
+      <c r="D10" t="s" s="10">
         <v>30</v>
-      </c>
-      <c r="D10" t="s" s="10">
-        <v>31</v>
       </c>
       <c r="E10" s="7"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
       <c r="A11" t="s" s="8">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s" s="9">
         <v>5</v>
       </c>
       <c r="C11" t="s" s="10">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s" s="10">
         <v>33</v>
-      </c>
-      <c r="D11" t="s" s="10">
-        <v>34</v>
       </c>
       <c r="E11" s="7"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
       <c r="A12" t="s" s="8">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s" s="9">
         <v>5</v>
       </c>
       <c r="C12" t="s" s="10">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s" s="10">
         <v>36</v>
-      </c>
-      <c r="D12" t="s" s="10">
-        <v>37</v>
       </c>
       <c r="E12" s="7"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
       <c r="A13" t="s" s="8">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s" s="9">
         <v>38</v>
       </c>
-      <c r="B13" t="s" s="9">
+      <c r="C13" t="s" s="10">
         <v>39</v>
       </c>
-      <c r="C13" t="s" s="10">
+      <c r="D13" t="s" s="10">
         <v>40</v>
-      </c>
-      <c r="D13" t="s" s="10">
-        <v>41</v>
       </c>
       <c r="E13" s="7"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
       <c r="A14" t="s" s="8">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s" s="9">
         <v>5</v>
       </c>
       <c r="C14" t="s" s="10">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s" s="10">
         <v>43</v>
-      </c>
-      <c r="D14" t="s" s="10">
-        <v>44</v>
       </c>
       <c r="E14" s="7"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
       <c r="A15" t="s" s="8">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s" s="9">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s" s="10">
         <v>45</v>
       </c>
-      <c r="B15" t="s" s="9">
-        <v>39</v>
-      </c>
-      <c r="C15" t="s" s="10">
+      <c r="D15" t="s" s="10">
         <v>46</v>
-      </c>
-      <c r="D15" t="s" s="10">
-        <v>47</v>
       </c>
       <c r="E15" s="7"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
       <c r="A16" t="s" s="8">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s" s="9">
         <v>5</v>
       </c>
       <c r="C16" t="s" s="10">
+        <v>48</v>
+      </c>
+      <c r="D16" t="s" s="10">
         <v>49</v>
-      </c>
-      <c r="D16" t="s" s="10">
-        <v>50</v>
       </c>
       <c r="E16" s="7"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
       <c r="A17" t="s" s="8">
+        <v>50</v>
+      </c>
+      <c r="B17" t="s" s="9">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s" s="10">
         <v>51</v>
       </c>
-      <c r="B17" t="s" s="9">
-        <v>39</v>
-      </c>
-      <c r="C17" t="s" s="10">
+      <c r="D17" t="s" s="10">
         <v>52</v>
-      </c>
-      <c r="D17" t="s" s="10">
-        <v>53</v>
       </c>
       <c r="E17" s="7"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
       <c r="A18" t="s" s="8">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B18" t="s" s="9">
         <v>5</v>
       </c>
       <c r="C18" t="s" s="10">
+        <v>54</v>
+      </c>
+      <c r="D18" t="s" s="10">
         <v>55</v>
-      </c>
-      <c r="D18" t="s" s="10">
-        <v>56</v>
       </c>
       <c r="E18" s="7"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
       <c r="A19" t="s" s="8">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B19" t="s" s="9">
         <v>17</v>
@@ -1863,73 +1860,73 @@
         <v>18</v>
       </c>
       <c r="D19" t="s" s="10">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E19" s="7"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
       <c r="A20" t="s" s="8">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" t="s" s="9">
         <v>5</v>
       </c>
       <c r="C20" t="s" s="10">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D20" t="s" s="10">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E20" s="7"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
       <c r="A21" t="s" s="8">
+        <v>60</v>
+      </c>
+      <c r="B21" t="s" s="9">
         <v>61</v>
       </c>
-      <c r="B21" t="s" s="9">
+      <c r="C21" t="s" s="10">
         <v>62</v>
       </c>
-      <c r="C21" t="s" s="10">
+      <c r="D21" t="s" s="10">
         <v>63</v>
-      </c>
-      <c r="D21" t="s" s="10">
-        <v>64</v>
       </c>
       <c r="E21" s="7"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
       <c r="A22" t="s" s="8">
+        <v>64</v>
+      </c>
+      <c r="B22" t="s" s="9">
+        <v>38</v>
+      </c>
+      <c r="C22" t="s" s="10">
         <v>65</v>
       </c>
-      <c r="B22" t="s" s="9">
-        <v>39</v>
-      </c>
-      <c r="C22" t="s" s="10">
+      <c r="D22" t="s" s="10">
         <v>66</v>
-      </c>
-      <c r="D22" t="s" s="10">
-        <v>67</v>
       </c>
       <c r="E22" s="7"/>
     </row>
     <row r="23" ht="20.05" customHeight="1">
       <c r="A23" t="s" s="8">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s" s="9">
         <v>5</v>
       </c>
       <c r="C23" t="s" s="10">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D23" t="s" s="10">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E23" s="7"/>
     </row>
     <row r="24" ht="20.05" customHeight="1">
       <c r="A24" t="s" s="8">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B24" t="s" s="9">
         <v>5</v>
@@ -1938,37 +1935,37 @@
         <v>6</v>
       </c>
       <c r="D24" t="s" s="10">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E24" s="7"/>
     </row>
     <row r="25" ht="20.05" customHeight="1">
       <c r="A25" t="s" s="8">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B25" t="s" s="9">
         <v>5</v>
       </c>
       <c r="C25" t="s" s="10">
+        <v>72</v>
+      </c>
+      <c r="D25" t="s" s="10">
         <v>73</v>
-      </c>
-      <c r="D25" t="s" s="10">
-        <v>74</v>
       </c>
       <c r="E25" s="11"/>
     </row>
     <row r="26" ht="20.05" customHeight="1">
       <c r="A26" t="s" s="8">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B26" t="s" s="9">
         <v>17</v>
       </c>
       <c r="C26" t="s" s="10">
+        <v>75</v>
+      </c>
+      <c r="D26" t="s" s="10">
         <v>76</v>
-      </c>
-      <c r="D26" t="s" s="10">
-        <v>77</v>
       </c>
       <c r="E26" s="12"/>
     </row>

</xml_diff>